<commit_message>
add new 2 testcases
</commit_message>
<xml_diff>
--- a/QA_TestData.xlsx
+++ b/QA_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12876" windowHeight="5208" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewTestCases" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7505" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7542" uniqueCount="1116">
   <si>
     <t>TestCase</t>
   </si>
@@ -3391,6 +3391,24 @@
   </si>
   <si>
     <t>VerifyThatUserRedirectOnSameTopicCardWhichWasSelected</t>
+  </si>
+  <si>
+    <t>Verify_That_SearchOrAskSomething_Option_Redirects_To_At_Home_Page</t>
+  </si>
+  <si>
+    <t>ClickOnSearchAndAksQuestionOption</t>
+  </si>
+  <si>
+    <t>Verify_That_User_Can_Switch_SearchOrAskSomething_To_FillOutAnRFI_Option_Witchout_Again_Login</t>
+  </si>
+  <si>
+    <t>VerifyThatUserCanSwitchSearchOrAskSomethingToFillOutAnRFIOptionWitchoutAgainLogin</t>
+  </si>
+  <si>
+    <t>Verify_That_User_Can_Switch_FillOutAnRFI_To_SearchOrAskSomething_Option_Witchout_Again_Login</t>
+  </si>
+  <si>
+    <t>VerifyThatUserCanSwitchFillOutAnRFIToSearchOrAskSomethingOptionWitchoutAgainLogin</t>
   </si>
 </sst>
 </file>
@@ -4161,10 +4179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V211"/>
+  <dimension ref="A1:V214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="E222" sqref="E222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -11257,6 +11275,78 @@
         <v>6</v>
       </c>
     </row>
+    <row r="212" spans="1:11" ht="28.8">
+      <c r="A212" s="7" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C212" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E212" s="31" t="s">
+        <v>559</v>
+      </c>
+      <c r="F212" s="31" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G212" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="H212" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" ht="43.2">
+      <c r="A213" s="7" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D213" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E213" s="31" t="s">
+        <v>559</v>
+      </c>
+      <c r="F213" s="7" t="s">
+        <v>1113</v>
+      </c>
+      <c r="G213" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" ht="43.2">
+      <c r="A214" s="7" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D214" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E214" s="31" t="s">
+        <v>559</v>
+      </c>
+      <c r="F214" s="7" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G214" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:S1"/>
@@ -11268,11 +11358,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC387"/>
+  <dimension ref="A1:AC390"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A379" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E390" sqref="E390"/>
+      <selection pane="bottomLeft" activeCell="G385" sqref="G385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20945,6 +21035,57 @@
         <v>761</v>
       </c>
     </row>
+    <row r="388" spans="1:17" ht="28.8">
+      <c r="A388" s="7" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B388" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C388" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D388" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E388" s="63" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="389" spans="1:17" ht="43.2">
+      <c r="A389" s="7" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B389" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C389" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D389" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E389" s="63" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="390" spans="1:17" ht="43.2">
+      <c r="A390" s="7" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B390" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C390" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D390" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E390" s="63" t="s">
+        <v>761</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
@@ -20954,7 +21095,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E328">
       <formula1>"Market Research,Regs and Policies,Product Support,IEEE Data"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E358:E387">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E358:E390">
       <formula1>"Market Research,Regs and Policies,Product Support,Chinook"</formula1>
     </dataValidation>
   </dataValidations>
@@ -21525,9 +21666,15 @@
     <hyperlink ref="D386" r:id="rId564"/>
     <hyperlink ref="C387" r:id="rId565"/>
     <hyperlink ref="D387" r:id="rId566"/>
+    <hyperlink ref="C388" r:id="rId567"/>
+    <hyperlink ref="D388" r:id="rId568"/>
+    <hyperlink ref="C389" r:id="rId569"/>
+    <hyperlink ref="D389" r:id="rId570"/>
+    <hyperlink ref="C390" r:id="rId571"/>
+    <hyperlink ref="D390" r:id="rId572"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId567"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId573"/>
 </worksheet>
 </file>
 

</xml_diff>